<commit_message>
Edit plan, test cases, and checklist
</commit_message>
<xml_diff>
--- a/CheckMalashenko.xlsx
+++ b/CheckMalashenko.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Евгения\Desktop\netology\Тестирование\ДИПЛОМ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects with JaCoCo\QAdiplom2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED329DE9-361C-4D3C-92C7-07049AC6CA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4688275C-870E-4629-8526-448B43EDC736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="67">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -169,6 +169,63 @@
   </si>
   <si>
     <t>Приложение "В Хосписе"</t>
+  </si>
+  <si>
+    <t>Производительность</t>
+  </si>
+  <si>
+    <t>Нагрузочное тестирование - проверка работоспособности приложения при большом количестве авторизаций пользователя</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Конфигурационное тестирование. Проверяется, корректно ли работает приложение в разных средах, на различных устройствах и операционных системах.</t>
+  </si>
+  <si>
+    <t>Локализация. Вход в приложение в разных странах и корректность отображения содержимого</t>
+  </si>
+  <si>
+    <t>Работа приложения на нескольких устройствах  с одного аккаунта одновременно</t>
+  </si>
+  <si>
+    <t>Не проводилось еще</t>
+  </si>
+  <si>
+    <t>Проверка работы приложения и его скорости в разных условиях (при медленном соединении интернета, при потере сигнала интернета, в метро, на высоте, в лифте, при изменении погодных условий, при подключении к wi-fi, при использовании мобильного интернета, при использовании зарядного устройства, в режиме "авиа")</t>
+  </si>
+  <si>
+    <t>пройден</t>
+  </si>
+  <si>
+    <t>Безопасность</t>
+  </si>
+  <si>
+    <t>Проверка уязвимостей приложения на предмет взлома и утечки данных</t>
+  </si>
+  <si>
+    <t>Удобство использования (UX/UI)</t>
+  </si>
+  <si>
+    <t>Поведение приложения при повороте устройства</t>
+  </si>
+  <si>
+    <t>Поведение приложения при встряхивании устройства</t>
+  </si>
+  <si>
+    <t>Светлая/темная темы</t>
+  </si>
+  <si>
+    <t>Определение функциональности всех кнопок/клавиш устройства. Кнопки/клавиши, не ассоциированные с функциями приложения, не вызывают неожиданного поведения при активации.</t>
+  </si>
+  <si>
+    <t>Ввод в поле "категория" текста вручную, не выбирая имеющиеся</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создание новости с пустыми полями </t>
+  </si>
+  <si>
+    <t>Выбор несуществующего времени вручную при создании новости</t>
   </si>
 </sst>
 </file>
@@ -248,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -373,12 +430,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -398,41 +492,71 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -715,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,12 +854,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -752,228 +876,228 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16"/>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="15" t="s">
+      <c r="C20" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>42</v>
       </c>
       <c r="E20" t="s">
@@ -981,132 +1105,296 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="C21" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
+      <c r="B22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
+      <c r="B23" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="15"/>
+      <c r="B24" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13"/>
-      <c r="B23" s="18" t="s">
+      <c r="C25" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="15"/>
+      <c r="B26" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="15" t="s">
+      <c r="C26" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13"/>
-      <c r="B24" s="18" t="s">
+    <row r="27" spans="1:5" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="15"/>
+      <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="15" t="s">
+      <c r="C27" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="16"/>
-      <c r="B25" s="18" t="s">
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="16"/>
+      <c r="B28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+      <c r="C28" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C29" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16"/>
-      <c r="B27" s="18" t="s">
+      <c r="D29" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="16"/>
+      <c r="B30" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
+      <c r="D30" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
-      <c r="B29" s="6" t="s">
+      <c r="C31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="C32" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="23"/>
+      <c r="B34" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="23"/>
+      <c r="B35" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="23"/>
+      <c r="B36" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="23"/>
+      <c r="B37" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="19"/>
+      <c r="B40" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="19"/>
+      <c r="B41" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="18"/>
+      <c r="B42" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="27" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A39:A42"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A17:A24"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A14:A16"/>

</xml_diff>